<commit_message>
Updated several thesis resources
In this version, we added the following changes:
- Updated the source code of the three software systems: FRL, HRM and ORA.
- Updated the database dump files of the two software systems: FRL and HRM.
- Updated the installation manuals of the three software systems: FRL, HRM and ORA.
- Updated the results of the Evaluation
</commit_message>
<xml_diff>
--- a/Evaluation/Documents/Attack_Scenarios_OH.xlsx
+++ b/Evaluation/Documents/Attack_Scenarios_OH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Backup Plus/UCD/PHD/Approach/Evaluation/NEW/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F256A7-8DDD-C544-B558-8F338C24FC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9041B2C-C27F-814E-9308-2623AF6A0581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{0402DF6F-8EAC-0D4E-8631-6BF059FC1A8C}"/>
   </bookViews>
@@ -2060,7 +2060,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2100,12 +2100,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2291,7 +2285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2573,9 +2567,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2676,6 +2667,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2991,17 +2999,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A162E6D-53FB-BC41-A08E-35F51D53775C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O20" sqref="O20:O24"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="80" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="80" customWidth="1"/>
     <col min="2" max="2" width="16" style="80" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="81" customWidth="1"/>
     <col min="4" max="4" width="15" style="80" customWidth="1"/>
@@ -3087,51 +3094,51 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="76" x14ac:dyDescent="0.2">
-      <c r="A2" s="111">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="1:21" s="151" customFormat="1" ht="76" x14ac:dyDescent="0.2">
+      <c r="A2" s="145">
+        <v>1</v>
+      </c>
+      <c r="B2" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="146">
+        <v>1</v>
+      </c>
+      <c r="D2" s="145">
+        <v>1</v>
+      </c>
+      <c r="E2" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="145" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="145" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15" t="str">
+      <c r="J2" s="147" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="148"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
+      <c r="O2" s="148" t="str">
         <f>_xlfn.CONCAT(C2, "&amp;",B2,"&amp;",E2,"&amp;",F2,"&amp;",H2,"&amp;",N2,"&amp;","\\ \hline")</f>
         <v>1&amp;Incident&amp;OH&gt;Login&gt;&amp;A Doctor CONNECTS to the Open Hospital Software System &amp;physician&amp;&amp;\\ \hline</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
+      <c r="P2" s="145"/>
+      <c r="Q2" s="150"/>
+      <c r="R2" s="150"/>
+      <c r="S2" s="150"/>
+      <c r="T2" s="150"/>
+      <c r="U2" s="150"/>
     </row>
     <row r="3" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -4103,7 +4110,7 @@
       <c r="T24" s="79"/>
       <c r="U24" s="79"/>
     </row>
-    <row r="25" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
         <v>2</v>
       </c>
@@ -4146,7 +4153,7 @@
       <c r="T25" s="9"/>
       <c r="U25" s="9"/>
     </row>
-    <row r="26" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -4185,7 +4192,7 @@
       <c r="T26" s="9"/>
       <c r="U26" s="9"/>
     </row>
-    <row r="27" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -4224,7 +4231,7 @@
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
     </row>
-    <row r="28" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -4263,7 +4270,7 @@
       <c r="T28" s="79"/>
       <c r="U28" s="79"/>
     </row>
-    <row r="29" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
         <v>2</v>
       </c>
@@ -4306,7 +4313,7 @@
       <c r="T29" s="9"/>
       <c r="U29" s="9"/>
     </row>
-    <row r="30" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -4345,7 +4352,7 @@
       <c r="T30" s="9"/>
       <c r="U30" s="9"/>
     </row>
-    <row r="31" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -4384,7 +4391,7 @@
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
     </row>
-    <row r="32" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <v>2</v>
       </c>
@@ -4423,7 +4430,7 @@
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
     </row>
-    <row r="33" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -4462,7 +4469,7 @@
       <c r="T33" s="9"/>
       <c r="U33" s="9"/>
     </row>
-    <row r="34" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
         <v>2</v>
       </c>
@@ -4505,7 +4512,7 @@
       <c r="T34" s="9"/>
       <c r="U34" s="9"/>
     </row>
-    <row r="35" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
         <v>2</v>
       </c>
@@ -4546,7 +4553,7 @@
       <c r="T35" s="9"/>
       <c r="U35" s="9"/>
     </row>
-    <row r="36" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -4585,7 +4592,7 @@
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
     </row>
-    <row r="37" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -4624,7 +4631,7 @@
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
     </row>
-    <row r="38" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -4663,7 +4670,7 @@
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
     </row>
-    <row r="39" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A39" s="14">
         <v>2</v>
       </c>
@@ -4720,7 +4727,7 @@
       </c>
       <c r="U39" s="9"/>
     </row>
-    <row r="40" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -4759,7 +4766,7 @@
       <c r="T40" s="9"/>
       <c r="U40" s="9"/>
     </row>
-    <row r="41" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -4798,7 +4805,7 @@
       <c r="T41" s="9"/>
       <c r="U41" s="9"/>
     </row>
-    <row r="42" spans="1:21" s="6" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" s="6" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>2</v>
       </c>
@@ -4837,7 +4844,7 @@
       <c r="T42" s="8"/>
       <c r="U42" s="8"/>
     </row>
-    <row r="43" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2</v>
       </c>
@@ -4876,7 +4883,7 @@
       <c r="T43" s="9"/>
       <c r="U43" s="9"/>
     </row>
-    <row r="44" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -4915,7 +4922,7 @@
       <c r="T44" s="9"/>
       <c r="U44" s="9"/>
     </row>
-    <row r="45" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2</v>
       </c>
@@ -4954,7 +4961,7 @@
       <c r="T45" s="9"/>
       <c r="U45" s="9"/>
     </row>
-    <row r="46" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A46" s="14">
         <v>2</v>
       </c>
@@ -4995,7 +5002,7 @@
       <c r="T46" s="9"/>
       <c r="U46" s="9"/>
     </row>
-    <row r="47" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A47" s="14">
         <v>3</v>
       </c>
@@ -5050,7 +5057,7 @@
       </c>
       <c r="U47" s="9"/>
     </row>
-    <row r="48" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>3</v>
       </c>
@@ -5089,7 +5096,7 @@
       <c r="T48" s="9"/>
       <c r="U48" s="9"/>
     </row>
-    <row r="49" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -5128,7 +5135,7 @@
       <c r="T49" s="9"/>
       <c r="U49" s="9"/>
     </row>
-    <row r="50" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -5167,7 +5174,7 @@
       <c r="T50" s="9"/>
       <c r="U50" s="9"/>
     </row>
-    <row r="51" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>3</v>
       </c>
@@ -5206,7 +5213,7 @@
       <c r="T51" s="9"/>
       <c r="U51" s="9"/>
     </row>
-    <row r="52" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A52" s="14">
         <v>3</v>
       </c>
@@ -5261,7 +5268,7 @@
       </c>
       <c r="U52" s="9"/>
     </row>
-    <row r="53" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -5300,7 +5307,7 @@
       <c r="T53" s="9"/>
       <c r="U53" s="9"/>
     </row>
-    <row r="54" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>3</v>
       </c>
@@ -5339,7 +5346,7 @@
       <c r="T54" s="9"/>
       <c r="U54" s="9"/>
     </row>
-    <row r="55" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -5378,7 +5385,7 @@
       <c r="T55" s="9"/>
       <c r="U55" s="9"/>
     </row>
-    <row r="56" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>3</v>
       </c>
@@ -5417,7 +5424,7 @@
       <c r="T56" s="9"/>
       <c r="U56" s="9"/>
     </row>
-    <row r="57" spans="1:21" s="6" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" s="6" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>3</v>
       </c>
@@ -5472,7 +5479,7 @@
       </c>
       <c r="U57" s="8"/>
     </row>
-    <row r="58" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>3</v>
       </c>
@@ -5511,7 +5518,7 @@
       <c r="T58" s="9"/>
       <c r="U58" s="9"/>
     </row>
-    <row r="59" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -5550,7 +5557,7 @@
       <c r="T59" s="9"/>
       <c r="U59" s="9"/>
     </row>
-    <row r="60" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -5589,7 +5596,7 @@
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
     </row>
-    <row r="61" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -5628,7 +5635,7 @@
       <c r="T61" s="9"/>
       <c r="U61" s="9"/>
     </row>
-    <row r="62" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A62" s="14">
         <v>3</v>
       </c>
@@ -5683,7 +5690,7 @@
       </c>
       <c r="U62" s="9"/>
     </row>
-    <row r="63" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -5722,7 +5729,7 @@
       <c r="T63" s="9"/>
       <c r="U63" s="9"/>
     </row>
-    <row r="64" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>3</v>
       </c>
@@ -5760,7 +5767,7 @@
       <c r="T64" s="9"/>
       <c r="U64" s="9"/>
     </row>
-    <row r="65" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>3</v>
       </c>
@@ -5799,7 +5806,7 @@
       <c r="T65" s="9"/>
       <c r="U65" s="9"/>
     </row>
-    <row r="66" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -5838,7 +5845,7 @@
       <c r="T66" s="9"/>
       <c r="U66" s="9"/>
     </row>
-    <row r="67" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>3</v>
       </c>
@@ -5877,7 +5884,7 @@
       <c r="T67" s="9"/>
       <c r="U67" s="9"/>
     </row>
-    <row r="68" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A68" s="14">
         <v>3</v>
       </c>
@@ -5932,7 +5939,7 @@
       </c>
       <c r="U68" s="9"/>
     </row>
-    <row r="69" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A69" s="14">
         <v>4</v>
       </c>
@@ -5973,7 +5980,7 @@
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
     </row>
-    <row r="70" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>4</v>
       </c>
@@ -6012,7 +6019,7 @@
       <c r="T70" s="9"/>
       <c r="U70" s="9"/>
     </row>
-    <row r="71" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>4</v>
       </c>
@@ -6051,7 +6058,7 @@
       <c r="T71" s="9"/>
       <c r="U71" s="9"/>
     </row>
-    <row r="72" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>4</v>
       </c>
@@ -6090,7 +6097,7 @@
       <c r="T72" s="9"/>
       <c r="U72" s="9"/>
     </row>
-    <row r="73" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A73" s="14">
         <v>4</v>
       </c>
@@ -6131,7 +6138,7 @@
       <c r="T73" s="9"/>
       <c r="U73" s="9"/>
     </row>
-    <row r="74" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>4</v>
       </c>
@@ -6170,7 +6177,7 @@
       <c r="T74" s="9"/>
       <c r="U74" s="9"/>
     </row>
-    <row r="75" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <v>4</v>
       </c>
@@ -6209,7 +6216,7 @@
       <c r="T75" s="9"/>
       <c r="U75" s="9"/>
     </row>
-    <row r="76" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>4</v>
       </c>
@@ -6248,7 +6255,7 @@
       <c r="T76" s="9"/>
       <c r="U76" s="9"/>
     </row>
-    <row r="77" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>4</v>
       </c>
@@ -6287,7 +6294,7 @@
       <c r="T77" s="9"/>
       <c r="U77" s="9"/>
     </row>
-    <row r="78" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A78" s="14">
         <v>4</v>
       </c>
@@ -6328,7 +6335,7 @@
       <c r="T78" s="9"/>
       <c r="U78" s="9"/>
     </row>
-    <row r="79" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A79" s="14">
         <v>4</v>
       </c>
@@ -6383,7 +6390,7 @@
       </c>
       <c r="U79" s="9"/>
     </row>
-    <row r="80" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>4</v>
       </c>
@@ -6422,7 +6429,7 @@
       <c r="T80" s="9"/>
       <c r="U80" s="9"/>
     </row>
-    <row r="81" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>4</v>
       </c>
@@ -6461,7 +6468,7 @@
       <c r="T81" s="9"/>
       <c r="U81" s="9"/>
     </row>
-    <row r="82" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>4</v>
       </c>
@@ -6500,7 +6507,7 @@
       <c r="T82" s="9"/>
       <c r="U82" s="9"/>
     </row>
-    <row r="83" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>4</v>
       </c>
@@ -6539,7 +6546,7 @@
       <c r="T83" s="9"/>
       <c r="U83" s="9"/>
     </row>
-    <row r="84" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>4</v>
       </c>
@@ -6578,7 +6585,7 @@
       <c r="T84" s="9"/>
       <c r="U84" s="9"/>
     </row>
-    <row r="85" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A85" s="14">
         <v>4</v>
       </c>
@@ -6633,7 +6640,7 @@
       </c>
       <c r="U85" s="9"/>
     </row>
-    <row r="86" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>4</v>
       </c>
@@ -6672,7 +6679,7 @@
       <c r="T86" s="9"/>
       <c r="U86" s="9"/>
     </row>
-    <row r="87" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A87" s="18">
         <v>4</v>
       </c>
@@ -6711,7 +6718,7 @@
       <c r="T87" s="9"/>
       <c r="U87" s="9"/>
     </row>
-    <row r="88" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>4</v>
       </c>
@@ -6750,7 +6757,7 @@
       <c r="T88" s="9"/>
       <c r="U88" s="9"/>
     </row>
-    <row r="89" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>4</v>
       </c>
@@ -6789,7 +6796,7 @@
       <c r="T89" s="9"/>
       <c r="U89" s="9"/>
     </row>
-    <row r="90" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A90" s="14">
         <v>4</v>
       </c>
@@ -6844,7 +6851,7 @@
       </c>
       <c r="U90" s="9"/>
     </row>
-    <row r="91" spans="1:21" s="2" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" s="2" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A91" s="14">
         <v>5</v>
       </c>
@@ -6885,7 +6892,7 @@
       <c r="T91" s="3"/>
       <c r="U91" s="3"/>
     </row>
-    <row r="92" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>5</v>
       </c>
@@ -6924,7 +6931,7 @@
       <c r="T92" s="9"/>
       <c r="U92" s="9"/>
     </row>
-    <row r="93" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>5</v>
       </c>
@@ -6963,7 +6970,7 @@
       <c r="T93" s="9"/>
       <c r="U93" s="9"/>
     </row>
-    <row r="94" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>5</v>
       </c>
@@ -7002,7 +7009,7 @@
       <c r="T94" s="9"/>
       <c r="U94" s="9"/>
     </row>
-    <row r="95" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -7041,7 +7048,7 @@
       <c r="T95" s="9"/>
       <c r="U95" s="9"/>
     </row>
-    <row r="96" spans="1:21" s="2" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" s="2" customFormat="1" ht="38" x14ac:dyDescent="0.25">
       <c r="A96" s="14">
         <v>5</v>
       </c>
@@ -7082,7 +7089,7 @@
       <c r="T96" s="3"/>
       <c r="U96" s="3"/>
     </row>
-    <row r="97" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>5</v>
       </c>
@@ -7121,7 +7128,7 @@
       <c r="T97" s="9"/>
       <c r="U97" s="9"/>
     </row>
-    <row r="98" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>5</v>
       </c>
@@ -7160,7 +7167,7 @@
       <c r="T98" s="9"/>
       <c r="U98" s="9"/>
     </row>
-    <row r="99" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A99" s="18">
         <v>5</v>
       </c>
@@ -7199,7 +7206,7 @@
       <c r="T99" s="8"/>
       <c r="U99" s="8"/>
     </row>
-    <row r="100" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>5</v>
       </c>
@@ -7238,7 +7245,7 @@
       <c r="T100" s="9"/>
       <c r="U100" s="9"/>
     </row>
-    <row r="101" spans="1:21" s="2" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" s="2" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A101" s="14">
         <v>5</v>
       </c>
@@ -7279,7 +7286,7 @@
       <c r="T101" s="3"/>
       <c r="U101" s="3"/>
     </row>
-    <row r="102" spans="1:21" s="2" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" s="2" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A102" s="14">
         <v>5</v>
       </c>
@@ -7320,7 +7327,7 @@
       <c r="T102" s="3"/>
       <c r="U102" s="3"/>
     </row>
-    <row r="103" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>5</v>
       </c>
@@ -7359,7 +7366,7 @@
       <c r="T103" s="9"/>
       <c r="U103" s="9"/>
     </row>
-    <row r="104" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>5</v>
       </c>
@@ -7398,7 +7405,7 @@
       <c r="T104" s="9"/>
       <c r="U104" s="9"/>
     </row>
-    <row r="105" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>5</v>
       </c>
@@ -7437,7 +7444,7 @@
       <c r="T105" s="9"/>
       <c r="U105" s="9"/>
     </row>
-    <row r="106" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>5</v>
       </c>
@@ -7476,7 +7483,7 @@
       <c r="T106" s="9"/>
       <c r="U106" s="9"/>
     </row>
-    <row r="107" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>5</v>
       </c>
@@ -7515,7 +7522,7 @@
       <c r="T107" s="9"/>
       <c r="U107" s="9"/>
     </row>
-    <row r="108" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>5</v>
       </c>
@@ -7554,7 +7561,7 @@
       <c r="T108" s="9"/>
       <c r="U108" s="9"/>
     </row>
-    <row r="109" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>5</v>
       </c>
@@ -7593,7 +7600,7 @@
       <c r="T109" s="9"/>
       <c r="U109" s="9"/>
     </row>
-    <row r="110" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1">
@@ -7626,7 +7633,7 @@
       <c r="T110" s="9"/>
       <c r="U110" s="9"/>
     </row>
-    <row r="111" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>5</v>
       </c>
@@ -7665,7 +7672,7 @@
       <c r="T111" s="9"/>
       <c r="U111" s="9"/>
     </row>
-    <row r="112" spans="1:21" s="2" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:21" s="2" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A112" s="14">
         <v>5</v>
       </c>
@@ -7720,7 +7727,7 @@
       </c>
       <c r="U112" s="3"/>
     </row>
-    <row r="113" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>5</v>
       </c>
@@ -7759,7 +7766,7 @@
       <c r="T113" s="9"/>
       <c r="U113" s="9"/>
     </row>
-    <row r="114" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A114" s="18">
         <v>5</v>
       </c>
@@ -7798,7 +7805,7 @@
       <c r="T114" s="8"/>
       <c r="U114" s="8"/>
     </row>
-    <row r="115" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>5</v>
       </c>
@@ -7837,7 +7844,7 @@
       <c r="T115" s="9"/>
       <c r="U115" s="9"/>
     </row>
-    <row r="116" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A116" s="14">
         <v>5</v>
       </c>
@@ -7878,7 +7885,7 @@
       <c r="T116" s="9"/>
       <c r="U116" s="9"/>
     </row>
-    <row r="117" spans="1:21" s="2" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:21" s="2" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A117" s="14">
         <v>6</v>
       </c>
@@ -7919,7 +7926,7 @@
       <c r="T117" s="3"/>
       <c r="U117" s="3"/>
     </row>
-    <row r="118" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>6</v>
       </c>
@@ -7958,7 +7965,7 @@
       <c r="T118" s="9"/>
       <c r="U118" s="9"/>
     </row>
-    <row r="119" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>6</v>
       </c>
@@ -7997,7 +8004,7 @@
       <c r="T119" s="9"/>
       <c r="U119" s="9"/>
     </row>
-    <row r="120" spans="1:21" s="2" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
         <v>6</v>
       </c>
@@ -8038,7 +8045,7 @@
       <c r="T120" s="3"/>
       <c r="U120" s="3"/>
     </row>
-    <row r="121" spans="1:21" ht="20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="20" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>6</v>
       </c>
@@ -8077,7 +8084,7 @@
       <c r="T121" s="9"/>
       <c r="U121" s="9"/>
     </row>
-    <row r="122" spans="1:21" ht="39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>6</v>
       </c>
@@ -8116,7 +8123,7 @@
       <c r="T122" s="9"/>
       <c r="U122" s="9"/>
     </row>
-    <row r="123" spans="1:21" s="6" customFormat="1" ht="20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A123" s="18">
         <v>6</v>
       </c>
@@ -8155,7 +8162,7 @@
       <c r="T123" s="8"/>
       <c r="U123" s="8"/>
     </row>
-    <row r="124" spans="1:21" ht="20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="20" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>6</v>
       </c>
@@ -8194,7 +8201,7 @@
       <c r="T124" s="9"/>
       <c r="U124" s="9"/>
     </row>
-    <row r="125" spans="1:21" s="2" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:21" s="2" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A125" s="14">
         <v>6</v>
       </c>
@@ -8233,7 +8240,7 @@
       <c r="T125" s="3"/>
       <c r="U125" s="3"/>
     </row>
-    <row r="126" spans="1:21" s="2" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:21" s="2" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A126" s="14">
         <v>6</v>
       </c>
@@ -8288,7 +8295,7 @@
       </c>
       <c r="U126" s="3"/>
     </row>
-    <row r="127" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>6</v>
       </c>
@@ -8327,7 +8334,7 @@
       <c r="T127" s="9"/>
       <c r="U127" s="9"/>
     </row>
-    <row r="128" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>6</v>
       </c>
@@ -8366,7 +8373,7 @@
       <c r="T128" s="9"/>
       <c r="U128" s="9"/>
     </row>
-    <row r="129" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>6</v>
       </c>
@@ -8405,7 +8412,7 @@
       <c r="T129" s="9"/>
       <c r="U129" s="9"/>
     </row>
-    <row r="130" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>6</v>
       </c>
@@ -8444,7 +8451,7 @@
       <c r="T130" s="9"/>
       <c r="U130" s="9"/>
     </row>
-    <row r="131" spans="1:21" s="2" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:21" s="2" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A131" s="14">
         <v>6</v>
       </c>
@@ -8499,7 +8506,7 @@
       </c>
       <c r="U131" s="3"/>
     </row>
-    <row r="132" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>6</v>
       </c>
@@ -8538,7 +8545,7 @@
       <c r="T132" s="9"/>
       <c r="U132" s="9"/>
     </row>
-    <row r="133" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>6</v>
       </c>
@@ -8577,7 +8584,7 @@
       <c r="T133" s="9"/>
       <c r="U133" s="9"/>
     </row>
-    <row r="134" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>6</v>
       </c>
@@ -8616,7 +8623,7 @@
       <c r="T134" s="9"/>
       <c r="U134" s="9"/>
     </row>
-    <row r="135" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>6</v>
       </c>
@@ -8655,7 +8662,7 @@
       <c r="T135" s="9"/>
       <c r="U135" s="9"/>
     </row>
-    <row r="136" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A136" s="18">
         <v>6</v>
       </c>
@@ -8694,7 +8701,7 @@
       <c r="T136" s="8"/>
       <c r="U136" s="8"/>
     </row>
-    <row r="137" spans="1:21" s="2" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:21" s="2" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A137" s="14">
         <v>6</v>
       </c>
@@ -8749,7 +8756,7 @@
       </c>
       <c r="U137" s="3"/>
     </row>
-    <row r="138" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>6</v>
       </c>
@@ -8788,7 +8795,7 @@
       <c r="T138" s="9"/>
       <c r="U138" s="9"/>
     </row>
-    <row r="139" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>6</v>
       </c>
@@ -8827,7 +8834,7 @@
       <c r="T139" s="9"/>
       <c r="U139" s="9"/>
     </row>
-    <row r="140" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A140" s="18">
         <v>6</v>
       </c>
@@ -8866,7 +8873,7 @@
       <c r="T140" s="8"/>
       <c r="U140" s="8"/>
     </row>
-    <row r="141" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>6</v>
       </c>
@@ -8905,7 +8912,7 @@
       <c r="T141" s="9"/>
       <c r="U141" s="9"/>
     </row>
-    <row r="142" spans="1:21" s="2" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:21" s="2" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A142" s="14">
         <v>6</v>
       </c>
@@ -8960,7 +8967,7 @@
       </c>
       <c r="U142" s="3"/>
     </row>
-    <row r="143" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A143" s="14">
         <v>7</v>
       </c>
@@ -9003,7 +9010,7 @@
       <c r="T143" s="9"/>
       <c r="U143" s="9"/>
     </row>
-    <row r="144" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>7</v>
       </c>
@@ -9044,7 +9051,7 @@
       <c r="T144" s="9"/>
       <c r="U144" s="9"/>
     </row>
-    <row r="145" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>7</v>
       </c>
@@ -9085,7 +9092,7 @@
       <c r="T145" s="9"/>
       <c r="U145" s="9"/>
     </row>
-    <row r="146" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A146" s="14">
         <v>7</v>
       </c>
@@ -9128,7 +9135,7 @@
       <c r="T146" s="9"/>
       <c r="U146" s="9"/>
     </row>
-    <row r="147" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>7</v>
       </c>
@@ -9169,7 +9176,7 @@
       <c r="T147" s="9"/>
       <c r="U147" s="9"/>
     </row>
-    <row r="148" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>7</v>
       </c>
@@ -9210,7 +9217,7 @@
       <c r="T148" s="9"/>
       <c r="U148" s="9"/>
     </row>
-    <row r="149" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>7</v>
       </c>
@@ -9251,7 +9258,7 @@
       <c r="T149" s="9"/>
       <c r="U149" s="9"/>
     </row>
-    <row r="150" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A150" s="18">
         <v>7</v>
       </c>
@@ -9292,7 +9299,7 @@
       <c r="T150" s="8"/>
       <c r="U150" s="8"/>
     </row>
-    <row r="151" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A151" s="14">
         <v>7</v>
       </c>
@@ -9335,7 +9342,7 @@
       <c r="T151" s="9"/>
       <c r="U151" s="9"/>
     </row>
-    <row r="152" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A152" s="14">
         <v>7</v>
       </c>
@@ -9378,7 +9385,7 @@
       <c r="T152" s="9"/>
       <c r="U152" s="9"/>
     </row>
-    <row r="153" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>7</v>
       </c>
@@ -9419,7 +9426,7 @@
       <c r="T153" s="9"/>
       <c r="U153" s="9"/>
     </row>
-    <row r="154" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>7</v>
       </c>
@@ -9460,7 +9467,7 @@
       <c r="T154" s="9"/>
       <c r="U154" s="9"/>
     </row>
-    <row r="155" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>7</v>
       </c>
@@ -9501,7 +9508,7 @@
       <c r="T155" s="9"/>
       <c r="U155" s="9"/>
     </row>
-    <row r="156" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>7</v>
       </c>
@@ -9542,7 +9549,7 @@
       <c r="T156" s="9"/>
       <c r="U156" s="9"/>
     </row>
-    <row r="157" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A157" s="14">
         <v>7</v>
       </c>
@@ -9599,7 +9606,7 @@
       </c>
       <c r="U157" s="9"/>
     </row>
-    <row r="158" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>7</v>
       </c>
@@ -9640,7 +9647,7 @@
       <c r="T158" s="9"/>
       <c r="U158" s="9"/>
     </row>
-    <row r="159" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>7</v>
       </c>
@@ -9681,7 +9688,7 @@
       <c r="T159" s="9"/>
       <c r="U159" s="9"/>
     </row>
-    <row r="160" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A160" s="18">
         <v>7</v>
       </c>
@@ -9722,7 +9729,7 @@
       <c r="T160" s="8"/>
       <c r="U160" s="8"/>
     </row>
-    <row r="161" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>7</v>
       </c>
@@ -9763,7 +9770,7 @@
       <c r="T161" s="9"/>
       <c r="U161" s="9"/>
     </row>
-    <row r="162" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A162" s="14">
         <v>7</v>
       </c>
@@ -9806,7 +9813,7 @@
       <c r="T162" s="9"/>
       <c r="U162" s="9"/>
     </row>
-    <row r="163" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A163" s="14">
         <v>8</v>
       </c>
@@ -9849,7 +9856,7 @@
       <c r="T163" s="9"/>
       <c r="U163" s="9"/>
     </row>
-    <row r="164" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>8</v>
       </c>
@@ -9890,7 +9897,7 @@
       <c r="T164" s="9"/>
       <c r="U164" s="9"/>
     </row>
-    <row r="165" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>8</v>
       </c>
@@ -9931,7 +9938,7 @@
       <c r="T165" s="9"/>
       <c r="U165" s="9"/>
     </row>
-    <row r="166" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="38" x14ac:dyDescent="0.25">
       <c r="A166" s="14">
         <v>8</v>
       </c>
@@ -9974,7 +9981,7 @@
       <c r="T166" s="9"/>
       <c r="U166" s="9"/>
     </row>
-    <row r="167" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>8</v>
       </c>
@@ -10015,7 +10022,7 @@
       <c r="T167" s="9"/>
       <c r="U167" s="9"/>
     </row>
-    <row r="168" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>8</v>
       </c>
@@ -10056,7 +10063,7 @@
       <c r="T168" s="9"/>
       <c r="U168" s="9"/>
     </row>
-    <row r="169" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>8</v>
       </c>
@@ -10097,7 +10104,7 @@
       <c r="T169" s="9"/>
       <c r="U169" s="9"/>
     </row>
-    <row r="170" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A170" s="18">
         <v>8</v>
       </c>
@@ -10138,7 +10145,7 @@
       <c r="T170" s="9"/>
       <c r="U170" s="9"/>
     </row>
-    <row r="171" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A171" s="14">
         <v>8</v>
       </c>
@@ -10181,7 +10188,7 @@
       <c r="T171" s="9"/>
       <c r="U171" s="9"/>
     </row>
-    <row r="172" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A172" s="14">
         <v>8</v>
       </c>
@@ -10238,7 +10245,7 @@
       </c>
       <c r="U172" s="9"/>
     </row>
-    <row r="173" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>8</v>
       </c>
@@ -10279,7 +10286,7 @@
       <c r="T173" s="9"/>
       <c r="U173" s="9"/>
     </row>
-    <row r="174" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>8</v>
       </c>
@@ -10320,7 +10327,7 @@
       <c r="T174" s="9"/>
       <c r="U174" s="9"/>
     </row>
-    <row r="175" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A175" s="14">
         <v>8</v>
       </c>
@@ -10377,7 +10384,7 @@
       </c>
       <c r="U175" s="9"/>
     </row>
-    <row r="176" spans="1:21" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>8</v>
       </c>
@@ -10418,7 +10425,7 @@
       <c r="T176" s="9"/>
       <c r="U176" s="9"/>
     </row>
-    <row r="177" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>8</v>
       </c>
@@ -10459,7 +10466,7 @@
       <c r="T177" s="9"/>
       <c r="U177" s="9"/>
     </row>
-    <row r="178" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A178" s="18">
         <v>8</v>
       </c>
@@ -10500,7 +10507,7 @@
       <c r="T178" s="9"/>
       <c r="U178" s="9"/>
     </row>
-    <row r="179" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A179" s="14">
         <v>8</v>
       </c>
@@ -10557,7 +10564,7 @@
       </c>
       <c r="U179" s="9"/>
     </row>
-    <row r="180" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>8</v>
       </c>
@@ -10598,7 +10605,7 @@
       <c r="T180" s="9"/>
       <c r="U180" s="9"/>
     </row>
-    <row r="181" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>8</v>
       </c>
@@ -10639,7 +10646,7 @@
       <c r="T181" s="9"/>
       <c r="U181" s="9"/>
     </row>
-    <row r="182" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>8</v>
       </c>
@@ -10680,7 +10687,7 @@
       <c r="T182" s="9"/>
       <c r="U182" s="9"/>
     </row>
-    <row r="183" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A183" s="18">
         <v>8</v>
       </c>
@@ -10721,7 +10728,7 @@
       <c r="T183" s="9"/>
       <c r="U183" s="9"/>
     </row>
-    <row r="184" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>8</v>
       </c>
@@ -10762,7 +10769,7 @@
       <c r="T184" s="9"/>
       <c r="U184" s="9"/>
     </row>
-    <row r="185" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A185" s="14">
         <v>8</v>
       </c>
@@ -10819,7 +10826,7 @@
       </c>
       <c r="U185" s="9"/>
     </row>
-    <row r="186" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A186" s="14">
         <v>9</v>
       </c>
@@ -10876,7 +10883,7 @@
       </c>
       <c r="U186" s="9"/>
     </row>
-    <row r="187" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>9</v>
       </c>
@@ -10917,7 +10924,7 @@
       <c r="T187" s="9"/>
       <c r="U187" s="9"/>
     </row>
-    <row r="188" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>9</v>
       </c>
@@ -10958,7 +10965,7 @@
       <c r="T188" s="9"/>
       <c r="U188" s="9"/>
     </row>
-    <row r="189" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>9</v>
       </c>
@@ -10999,7 +11006,7 @@
       <c r="T189" s="9"/>
       <c r="U189" s="9"/>
     </row>
-    <row r="190" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A190" s="14">
         <v>9</v>
       </c>
@@ -11056,7 +11063,7 @@
       </c>
       <c r="U190" s="9"/>
     </row>
-    <row r="191" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>9</v>
       </c>
@@ -11097,7 +11104,7 @@
       <c r="T191" s="9"/>
       <c r="U191" s="9"/>
     </row>
-    <row r="192" spans="1:21" s="6" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:21" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A192" s="18">
         <v>9</v>
       </c>
@@ -11138,7 +11145,7 @@
       <c r="T192" s="8"/>
       <c r="U192" s="8"/>
     </row>
-    <row r="193" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>9</v>
       </c>
@@ -11179,7 +11186,7 @@
       <c r="T193" s="9"/>
       <c r="U193" s="9"/>
     </row>
-    <row r="194" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>9</v>
       </c>
@@ -11220,7 +11227,7 @@
       <c r="T194" s="9"/>
       <c r="U194" s="9"/>
     </row>
-    <row r="195" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A195" s="14">
         <v>9</v>
       </c>
@@ -11277,7 +11284,7 @@
       </c>
       <c r="U195" s="9"/>
     </row>
-    <row r="196" spans="1:21" s="6" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:21" s="6" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A196" s="18">
         <v>9</v>
       </c>
@@ -11332,7 +11339,7 @@
       </c>
       <c r="U196" s="8"/>
     </row>
-    <row r="197" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A197" s="14">
         <v>9</v>
       </c>
@@ -11389,7 +11396,7 @@
       </c>
       <c r="U197" s="9"/>
     </row>
-    <row r="198" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A198" s="14">
         <v>9</v>
       </c>
@@ -11446,7 +11453,7 @@
       </c>
       <c r="U198" s="9"/>
     </row>
-    <row r="199" spans="1:21" ht="49" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:21" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>9</v>
       </c>
@@ -11487,7 +11494,7 @@
       <c r="T199" s="9"/>
       <c r="U199" s="9"/>
     </row>
-    <row r="200" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A200" s="14">
         <v>9</v>
       </c>
@@ -11544,7 +11551,7 @@
       </c>
       <c r="U200" s="9"/>
     </row>
-    <row r="201" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>9</v>
       </c>
@@ -11585,7 +11592,7 @@
       <c r="T201" s="9"/>
       <c r="U201" s="9"/>
     </row>
-    <row r="202" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A202" s="18">
         <v>9</v>
       </c>
@@ -11626,7 +11633,7 @@
       <c r="T202" s="9"/>
       <c r="U202" s="9"/>
     </row>
-    <row r="203" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>9</v>
       </c>
@@ -11667,7 +11674,7 @@
       <c r="T203" s="9"/>
       <c r="U203" s="9"/>
     </row>
-    <row r="204" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>9</v>
       </c>
@@ -11708,7 +11715,7 @@
       <c r="T204" s="9"/>
       <c r="U204" s="9"/>
     </row>
-    <row r="205" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A205" s="14">
         <v>9</v>
       </c>
@@ -11765,7 +11772,7 @@
       </c>
       <c r="U205" s="14"/>
     </row>
-    <row r="206" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A206" s="14">
         <v>9</v>
       </c>
@@ -11822,7 +11829,7 @@
       </c>
       <c r="U206" s="14"/>
     </row>
-    <row r="207" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>9</v>
       </c>
@@ -11863,7 +11870,7 @@
       <c r="T207" s="9"/>
       <c r="U207" s="9"/>
     </row>
-    <row r="208" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>9</v>
       </c>
@@ -11904,7 +11911,7 @@
       <c r="T208" s="9"/>
       <c r="U208" s="9"/>
     </row>
-    <row r="209" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A209" s="14">
         <v>9</v>
       </c>
@@ -11961,7 +11968,7 @@
       </c>
       <c r="U209" s="9"/>
     </row>
-    <row r="210" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A210" s="18">
         <v>9</v>
       </c>
@@ -12002,7 +12009,7 @@
       <c r="T210" s="9"/>
       <c r="U210" s="9"/>
     </row>
-    <row r="211" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>9</v>
       </c>
@@ -12043,7 +12050,7 @@
       <c r="T211" s="9"/>
       <c r="U211" s="9"/>
     </row>
-    <row r="212" spans="1:21" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>9</v>
       </c>
@@ -12084,7 +12091,7 @@
       <c r="T212" s="9"/>
       <c r="U212" s="9"/>
     </row>
-    <row r="213" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>9</v>
       </c>
@@ -12125,7 +12132,7 @@
       <c r="T213" s="9"/>
       <c r="U213" s="9"/>
     </row>
-    <row r="214" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A214" s="14">
         <v>9</v>
       </c>
@@ -12182,7 +12189,7 @@
       </c>
       <c r="U214" s="14"/>
     </row>
-    <row r="215" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A215" s="14">
         <v>10</v>
       </c>
@@ -12239,7 +12246,7 @@
       </c>
       <c r="U215"/>
     </row>
-    <row r="216" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>10</v>
       </c>
@@ -12280,7 +12287,7 @@
       <c r="T216" s="9"/>
       <c r="U216" s="9"/>
     </row>
-    <row r="217" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>10</v>
       </c>
@@ -12321,7 +12328,7 @@
       <c r="T217" s="9"/>
       <c r="U217" s="9"/>
     </row>
-    <row r="218" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>10</v>
       </c>
@@ -12362,7 +12369,7 @@
       <c r="T218" s="9"/>
       <c r="U218" s="9"/>
     </row>
-    <row r="219" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>10</v>
       </c>
@@ -12403,7 +12410,7 @@
       <c r="T219" s="9"/>
       <c r="U219" s="9"/>
     </row>
-    <row r="220" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>10</v>
       </c>
@@ -12460,7 +12467,7 @@
       </c>
       <c r="U220" s="9"/>
     </row>
-    <row r="221" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>10</v>
       </c>
@@ -12501,7 +12508,7 @@
       <c r="T221" s="53"/>
       <c r="U221" s="9"/>
     </row>
-    <row r="222" spans="1:21" s="6" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:21" s="6" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A222" s="18">
         <v>10</v>
       </c>
@@ -12542,7 +12549,7 @@
       <c r="T222" s="108"/>
       <c r="U222" s="8"/>
     </row>
-    <row r="223" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>10</v>
       </c>
@@ -12583,7 +12590,7 @@
       <c r="T223" s="53"/>
       <c r="U223" s="9"/>
     </row>
-    <row r="224" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A224" s="14">
         <v>10</v>
       </c>
@@ -12640,7 +12647,7 @@
       </c>
       <c r="U224" s="9"/>
     </row>
-    <row r="225" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A225" s="14">
         <v>10</v>
       </c>
@@ -12697,7 +12704,7 @@
       </c>
       <c r="U225" s="9"/>
     </row>
-    <row r="226" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>10</v>
       </c>
@@ -12738,7 +12745,7 @@
       <c r="T226" s="53"/>
       <c r="U226" s="9"/>
     </row>
-    <row r="227" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>10</v>
       </c>
@@ -12779,7 +12786,7 @@
       <c r="T227" s="53"/>
       <c r="U227" s="9"/>
     </row>
-    <row r="228" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>10</v>
       </c>
@@ -12820,7 +12827,7 @@
       <c r="T228" s="9"/>
       <c r="U228" s="9"/>
     </row>
-    <row r="229" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A229" s="14">
         <v>10</v>
       </c>
@@ -12877,7 +12884,7 @@
       </c>
       <c r="U229" s="54"/>
     </row>
-    <row r="230" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>10</v>
       </c>
@@ -12918,7 +12925,7 @@
       <c r="T230" s="53"/>
       <c r="U230" s="9"/>
     </row>
-    <row r="231" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>10</v>
       </c>
@@ -12959,7 +12966,7 @@
       <c r="T231" s="53"/>
       <c r="U231" s="9"/>
     </row>
-    <row r="232" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A232" s="18">
         <v>10</v>
       </c>
@@ -13000,7 +13007,7 @@
       <c r="T232" s="53"/>
       <c r="U232" s="9"/>
     </row>
-    <row r="233" spans="1:21" ht="38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:21" ht="38" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>10</v>
       </c>
@@ -13041,7 +13048,7 @@
       <c r="T233" s="53"/>
       <c r="U233" s="9"/>
     </row>
-    <row r="234" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A234" s="14">
         <v>10</v>
       </c>
@@ -13098,7 +13105,7 @@
       </c>
       <c r="U234" s="9"/>
     </row>
-    <row r="235" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A235" s="14">
         <v>10</v>
       </c>
@@ -13155,7 +13162,7 @@
       </c>
       <c r="U235" s="9"/>
     </row>
-    <row r="236" spans="1:21" s="4" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:21" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>10</v>
       </c>
@@ -13196,7 +13203,7 @@
       <c r="T236" s="25"/>
       <c r="U236" s="7"/>
     </row>
-    <row r="237" spans="1:21" s="4" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:21" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>10</v>
       </c>
@@ -13237,7 +13244,7 @@
       <c r="T237" s="25"/>
       <c r="U237" s="7"/>
     </row>
-    <row r="238" spans="1:21" s="4" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:21" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>10</v>
       </c>
@@ -13278,7 +13285,7 @@
       <c r="T238" s="25"/>
       <c r="U238" s="7"/>
     </row>
-    <row r="239" spans="1:21" s="4" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:21" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>10</v>
       </c>
@@ -13319,7 +13326,7 @@
       <c r="T239" s="25"/>
       <c r="U239" s="7"/>
     </row>
-    <row r="240" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A240" s="14">
         <v>10</v>
       </c>
@@ -13376,7 +13383,7 @@
       </c>
       <c r="U240" s="9"/>
     </row>
-    <row r="241" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>10</v>
       </c>
@@ -13417,7 +13424,7 @@
       <c r="T241" s="53"/>
       <c r="U241" s="9"/>
     </row>
-    <row r="242" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:21" ht="57" x14ac:dyDescent="0.2">
       <c r="A242" s="18">
         <v>10</v>
       </c>
@@ -13458,7 +13465,7 @@
       <c r="T242" s="9"/>
       <c r="U242" s="9"/>
     </row>
-    <row r="243" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:21" ht="19" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>10</v>
       </c>
@@ -13499,7 +13506,7 @@
       <c r="T243" s="53"/>
       <c r="U243" s="9"/>
     </row>
-    <row r="244" spans="1:21" s="4" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:21" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>10</v>
       </c>
@@ -13540,7 +13547,7 @@
       <c r="T244" s="55"/>
       <c r="U244" s="7"/>
     </row>
-    <row r="245" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:21" ht="114" x14ac:dyDescent="0.2">
       <c r="A245" s="14">
         <v>10</v>
       </c>
@@ -13597,7 +13604,7 @@
       </c>
       <c r="U245" s="9"/>
     </row>
-    <row r="246" spans="1:21" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:21" ht="171" x14ac:dyDescent="0.2">
       <c r="A246" s="14">
         <v>11</v>
       </c>
@@ -13654,7 +13661,7 @@
       </c>
       <c r="U246" s="14"/>
     </row>
-    <row r="247" spans="1:21" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:21" ht="171" x14ac:dyDescent="0.2">
       <c r="A247" s="14">
         <v>12</v>
       </c>
@@ -13712,13 +13719,7 @@
       <c r="U247" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U247" xr:uid="{9A162E6D-53FB-BC41-A08E-35F51D53775C}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U247" xr:uid="{9A162E6D-53FB-BC41-A08E-35F51D53775C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13727,12 +13728,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C342F7-6CFD-E049-9AAA-2BA2F34142FE}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -13751,13 +13752,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="171" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="117" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="117" t="s">
         <v>177</v>
       </c>
       <c r="D1" s="57" t="s">
@@ -13787,32 +13788,32 @@
       <c r="L1" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="118" t="s">
+      <c r="M1" s="117" t="s">
         <v>291</v>
       </c>
-      <c r="N1" s="118" t="s">
+      <c r="N1" s="117" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="121" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="120" t="s">
         <v>188</v>
       </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="123"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="122"/>
       <c r="L2" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="M2" s="120"/>
-      <c r="N2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="118"/>
     </row>
     <row r="3" spans="1:14" ht="171" x14ac:dyDescent="0.2">
       <c r="A3" s="60">
@@ -13836,19 +13837,19 @@
       <c r="G3" s="62">
         <v>32</v>
       </c>
-      <c r="H3" s="114">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:H13" si="0">D3+E3+F3+G3</f>
         <v>3910</v>
       </c>
-      <c r="I3" s="114">
+      <c r="I3" s="113">
         <f t="shared" ref="I3:I13" si="1">H3/1000</f>
         <v>3.91</v>
       </c>
-      <c r="J3" s="114">
+      <c r="J3" s="113">
         <f>H3/C3</f>
         <v>88.86363636363636</v>
       </c>
-      <c r="K3" s="114">
+      <c r="K3" s="113">
         <f>I3/C3</f>
         <v>8.8863636363636367E-2</v>
       </c>
@@ -13884,19 +13885,19 @@
       <c r="G4" s="62">
         <v>19</v>
       </c>
-      <c r="H4" s="114">
+      <c r="H4" s="113">
         <f t="shared" si="0"/>
         <v>3091</v>
       </c>
-      <c r="I4" s="114">
+      <c r="I4" s="113">
         <f t="shared" si="1"/>
         <v>3.0910000000000002</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="113">
         <f t="shared" ref="J4:J14" si="2">H4/C4</f>
         <v>134.39130434782609</v>
       </c>
-      <c r="K4" s="114">
+      <c r="K4" s="113">
         <f t="shared" ref="K4:K14" si="3">I4/C4</f>
         <v>0.13439130434782609</v>
       </c>
@@ -13932,19 +13933,19 @@
       <c r="G5" s="62">
         <v>15</v>
       </c>
-      <c r="H5" s="114">
+      <c r="H5" s="113">
         <f t="shared" si="0"/>
         <v>1579</v>
       </c>
-      <c r="I5" s="114">
+      <c r="I5" s="113">
         <f t="shared" si="1"/>
         <v>1.579</v>
       </c>
-      <c r="J5" s="114">
+      <c r="J5" s="113">
         <f t="shared" si="2"/>
         <v>75.19047619047619</v>
       </c>
-      <c r="K5" s="114">
+      <c r="K5" s="113">
         <f t="shared" si="3"/>
         <v>7.5190476190476183E-2</v>
       </c>
@@ -13980,19 +13981,19 @@
       <c r="G6" s="62">
         <v>31</v>
       </c>
-      <c r="H6" s="114">
+      <c r="H6" s="113">
         <f t="shared" si="0"/>
         <v>4878</v>
       </c>
-      <c r="I6" s="114">
+      <c r="I6" s="113">
         <f t="shared" si="1"/>
         <v>4.8780000000000001</v>
       </c>
-      <c r="J6" s="114">
+      <c r="J6" s="113">
         <f t="shared" si="2"/>
         <v>113.44186046511628</v>
       </c>
-      <c r="K6" s="114">
+      <c r="K6" s="113">
         <f t="shared" si="3"/>
         <v>0.11344186046511628</v>
       </c>
@@ -14028,19 +14029,19 @@
       <c r="G7" s="62">
         <v>23</v>
       </c>
-      <c r="H7" s="114">
+      <c r="H7" s="113">
         <f t="shared" si="0"/>
         <v>3280</v>
       </c>
-      <c r="I7" s="114">
+      <c r="I7" s="113">
         <f t="shared" si="1"/>
         <v>3.28</v>
       </c>
-      <c r="J7" s="114">
+      <c r="J7" s="113">
         <f t="shared" si="2"/>
         <v>126.15384615384616</v>
       </c>
-      <c r="K7" s="114">
+      <c r="K7" s="113">
         <f t="shared" si="3"/>
         <v>0.12615384615384614</v>
       </c>
@@ -14076,19 +14077,19 @@
       <c r="G8" s="62">
         <v>29</v>
       </c>
-      <c r="H8" s="114">
+      <c r="H8" s="113">
         <f t="shared" si="0"/>
         <v>4661</v>
       </c>
-      <c r="I8" s="114">
+      <c r="I8" s="113">
         <f t="shared" si="1"/>
         <v>4.6609999999999996</v>
       </c>
-      <c r="J8" s="114">
+      <c r="J8" s="113">
         <f t="shared" si="2"/>
         <v>155.36666666666667</v>
       </c>
-      <c r="K8" s="114">
+      <c r="K8" s="113">
         <f t="shared" si="3"/>
         <v>0.15536666666666665</v>
       </c>
@@ -14124,19 +14125,19 @@
       <c r="G9" s="62">
         <v>8</v>
       </c>
-      <c r="H9" s="114">
+      <c r="H9" s="113">
         <f t="shared" si="0"/>
         <v>4191</v>
       </c>
-      <c r="I9" s="114">
+      <c r="I9" s="113">
         <f t="shared" si="1"/>
         <v>4.1909999999999998</v>
       </c>
-      <c r="J9" s="114">
+      <c r="J9" s="113">
         <f t="shared" si="2"/>
         <v>232.83333333333334</v>
       </c>
-      <c r="K9" s="114">
+      <c r="K9" s="113">
         <f t="shared" si="3"/>
         <v>0.23283333333333334</v>
       </c>
@@ -14172,19 +14173,19 @@
       <c r="G10" s="62">
         <v>10</v>
       </c>
-      <c r="H10" s="114">
+      <c r="H10" s="113">
         <f t="shared" si="0"/>
         <v>3243</v>
       </c>
-      <c r="I10" s="114">
+      <c r="I10" s="113">
         <f t="shared" si="1"/>
         <v>3.2429999999999999</v>
       </c>
-      <c r="J10" s="114">
+      <c r="J10" s="113">
         <f t="shared" si="2"/>
         <v>154.42857142857142</v>
       </c>
-      <c r="K10" s="114">
+      <c r="K10" s="113">
         <f t="shared" si="3"/>
         <v>0.15442857142857142</v>
       </c>
@@ -14220,19 +14221,19 @@
       <c r="G11" s="62">
         <v>22</v>
       </c>
-      <c r="H11" s="114">
+      <c r="H11" s="113">
         <f t="shared" si="0"/>
         <v>4176</v>
       </c>
-      <c r="I11" s="114">
+      <c r="I11" s="113">
         <f t="shared" si="1"/>
         <v>4.1760000000000002</v>
       </c>
-      <c r="J11" s="114">
+      <c r="J11" s="113">
         <f t="shared" si="2"/>
         <v>122.82352941176471</v>
       </c>
-      <c r="K11" s="114">
+      <c r="K11" s="113">
         <f t="shared" si="3"/>
         <v>0.12282352941176471</v>
       </c>
@@ -14268,19 +14269,19 @@
       <c r="G12" s="62">
         <v>14</v>
       </c>
-      <c r="H12" s="114">
+      <c r="H12" s="113">
         <f t="shared" si="0"/>
         <v>3697</v>
       </c>
-      <c r="I12" s="114">
+      <c r="I12" s="113">
         <f t="shared" si="1"/>
         <v>3.6970000000000001</v>
       </c>
-      <c r="J12" s="114">
+      <c r="J12" s="113">
         <f t="shared" si="2"/>
         <v>246.46666666666667</v>
       </c>
-      <c r="K12" s="114">
+      <c r="K12" s="113">
         <f t="shared" si="3"/>
         <v>0.24646666666666667</v>
       </c>
@@ -14316,19 +14317,19 @@
       <c r="G13" s="62">
         <v>2</v>
       </c>
-      <c r="H13" s="114">
+      <c r="H13" s="113">
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="I13" s="114">
+      <c r="I13" s="113">
         <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="J13" s="114">
+      <c r="J13" s="113">
         <f t="shared" si="2"/>
         <v>366.66666666666669</v>
       </c>
-      <c r="K13" s="114">
+      <c r="K13" s="113">
         <f t="shared" si="3"/>
         <v>0.3666666666666667</v>
       </c>
@@ -14364,19 +14365,19 @@
       <c r="G14" s="62">
         <v>0</v>
       </c>
-      <c r="H14" s="114">
+      <c r="H14" s="113">
         <f t="shared" ref="H14" si="4">D14+E14+F14+G14</f>
         <v>1007</v>
       </c>
-      <c r="I14" s="114">
+      <c r="I14" s="113">
         <f t="shared" ref="I14" si="5">H14/1000</f>
         <v>1.0069999999999999</v>
       </c>
-      <c r="J14" s="114">
+      <c r="J14" s="113">
         <f t="shared" si="2"/>
         <v>503.5</v>
       </c>
-      <c r="K14" s="114">
+      <c r="K14" s="113">
         <f t="shared" si="3"/>
         <v>0.50349999999999995</v>
       </c>
@@ -14439,25 +14440,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="67" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="130" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="129" t="s">
+      <c r="C1" s="128" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="129" t="s">
+      <c r="D1" s="128" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="129" t="s">
+      <c r="E1" s="128" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="129" t="s">
+      <c r="F1" s="128" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="129" t="s">
+      <c r="G1" s="128" t="s">
         <v>195</v>
       </c>
       <c r="H1" s="65" t="s">
@@ -14496,53 +14497,53 @@
       <c r="S1" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="T1" s="137" t="s">
+      <c r="T1" s="136" t="s">
         <v>207</v>
       </c>
-      <c r="U1" s="138" t="s">
+      <c r="U1" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="V1" s="139"/>
+      <c r="V1" s="138"/>
       <c r="W1" s="66"/>
-      <c r="X1" s="124" t="s">
+      <c r="X1" s="123" t="s">
         <v>209</v>
       </c>
-      <c r="Y1" s="124" t="s">
+      <c r="Y1" s="123" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="70" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="130"/>
-      <c r="B2" s="132"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="142" t="s">
+      <c r="A2" s="129"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="141" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="144"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
+      <c r="O2" s="142"/>
+      <c r="P2" s="142"/>
+      <c r="Q2" s="143"/>
       <c r="R2" s="68" t="s">
         <v>211</v>
       </c>
       <c r="S2" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="T2" s="137"/>
-      <c r="U2" s="140"/>
-      <c r="V2" s="141"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="139"/>
+      <c r="V2" s="140"/>
       <c r="W2" s="69"/>
-      <c r="X2" s="124"/>
-      <c r="Y2" s="124"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
     </row>
     <row r="3" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -14584,19 +14585,19 @@
       <c r="M3" s="1">
         <v>3</v>
       </c>
-      <c r="N3" s="115">
+      <c r="N3" s="114">
         <f t="shared" ref="N3:N8" si="0">H3+I3+J3+K3+L3+M3</f>
         <v>115</v>
       </c>
-      <c r="O3" s="115">
+      <c r="O3" s="114">
         <f t="shared" ref="O3" si="1">N3/1000</f>
         <v>0.115</v>
       </c>
-      <c r="P3" s="115">
+      <c r="P3" s="114">
         <f>N3/F3</f>
         <v>38.333333333333336</v>
       </c>
-      <c r="Q3" s="115">
+      <c r="Q3" s="114">
         <f>O3/F3</f>
         <v>3.8333333333333337E-2</v>
       </c>
@@ -14609,11 +14610,11 @@
       <c r="T3" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="U3" s="135" t="s">
+      <c r="U3" s="134" t="s">
         <v>220</v>
       </c>
-      <c r="V3" s="145"/>
-      <c r="W3" s="136"/>
+      <c r="V3" s="144"/>
+      <c r="W3" s="135"/>
       <c r="X3" s="1" t="s">
         <v>281</v>
       </c>
@@ -14621,7 +14622,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="67" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="67" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -14661,19 +14662,19 @@
       <c r="M4" s="1">
         <v>2</v>
       </c>
-      <c r="N4" s="115">
+      <c r="N4" s="114">
         <f t="shared" si="0"/>
         <v>321</v>
       </c>
-      <c r="O4" s="115">
+      <c r="O4" s="114">
         <f t="shared" ref="O4:O5" si="2">N4/1000</f>
         <v>0.32100000000000001</v>
       </c>
-      <c r="P4" s="115">
+      <c r="P4" s="114">
         <f t="shared" ref="P4:P26" si="3">N4/F4</f>
         <v>14.590909090909092</v>
       </c>
-      <c r="Q4" s="115">
+      <c r="Q4" s="114">
         <f t="shared" ref="Q4:Q26" si="4">O4/F4</f>
         <v>1.4590909090909092E-2</v>
       </c>
@@ -14686,11 +14687,11 @@
       <c r="T4" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="U4" s="135" t="s">
+      <c r="U4" s="134" t="s">
         <v>247</v>
       </c>
-      <c r="V4" s="145"/>
-      <c r="W4" s="136"/>
+      <c r="V4" s="144"/>
+      <c r="W4" s="135"/>
       <c r="X4" s="1" t="s">
         <v>273</v>
       </c>
@@ -14736,19 +14737,19 @@
       <c r="M5" s="29">
         <v>0</v>
       </c>
-      <c r="N5" s="116">
+      <c r="N5" s="115">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="O5" s="116">
+      <c r="O5" s="115">
         <f t="shared" si="2"/>
         <v>0.13</v>
       </c>
-      <c r="P5" s="115">
+      <c r="P5" s="114">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="Q5" s="115">
+      <c r="Q5" s="114">
         <f t="shared" si="4"/>
         <v>6.5000000000000002E-2</v>
       </c>
@@ -14761,11 +14762,11 @@
       <c r="T5" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="U5" s="126" t="s">
+      <c r="U5" s="125" t="s">
         <v>229</v>
       </c>
-      <c r="V5" s="127"/>
-      <c r="W5" s="128"/>
+      <c r="V5" s="126"/>
+      <c r="W5" s="127"/>
       <c r="X5" s="1" t="s">
         <v>282</v>
       </c>
@@ -14813,19 +14814,19 @@
       <c r="M6" s="1">
         <v>0</v>
       </c>
-      <c r="N6" s="115">
+      <c r="N6" s="114">
         <f t="shared" si="0"/>
         <v>316</v>
       </c>
-      <c r="O6" s="115">
+      <c r="O6" s="114">
         <f t="shared" ref="O6:O7" si="5">N6/1000</f>
         <v>0.316</v>
       </c>
-      <c r="P6" s="115">
+      <c r="P6" s="114">
         <f t="shared" si="3"/>
         <v>24.307692307692307</v>
       </c>
-      <c r="Q6" s="115">
+      <c r="Q6" s="114">
         <f t="shared" si="4"/>
         <v>2.4307692307692308E-2</v>
       </c>
@@ -14838,11 +14839,11 @@
       <c r="T6" s="83" t="s">
         <v>233</v>
       </c>
-      <c r="U6" s="125" t="s">
+      <c r="U6" s="124" t="s">
         <v>248</v>
       </c>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125"/>
+      <c r="V6" s="124"/>
+      <c r="W6" s="124"/>
       <c r="X6" s="1" t="s">
         <v>272</v>
       </c>
@@ -14888,19 +14889,19 @@
       <c r="M7" s="1">
         <v>0</v>
       </c>
-      <c r="N7" s="115">
+      <c r="N7" s="114">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="O7" s="115">
+      <c r="O7" s="114">
         <f t="shared" si="5"/>
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="P7" s="115">
+      <c r="P7" s="114">
         <f t="shared" si="3"/>
         <v>10.75</v>
       </c>
-      <c r="Q7" s="115">
+      <c r="Q7" s="114">
         <f t="shared" si="4"/>
         <v>1.0749999999999999E-2</v>
       </c>
@@ -14913,15 +14914,15 @@
       <c r="T7" s="83" t="s">
         <v>242</v>
       </c>
-      <c r="U7" s="125" t="s">
+      <c r="U7" s="124" t="s">
         <v>246</v>
       </c>
-      <c r="V7" s="125"/>
-      <c r="W7" s="125"/>
+      <c r="V7" s="124"/>
+      <c r="W7" s="124"/>
       <c r="X7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="Y7" s="112" t="s">
+      <c r="Y7" s="111" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14965,19 +14966,19 @@
       <c r="M8" s="1">
         <v>0</v>
       </c>
-      <c r="N8" s="115">
+      <c r="N8" s="114">
         <f t="shared" si="0"/>
         <v>286</v>
       </c>
-      <c r="O8" s="115">
+      <c r="O8" s="114">
         <f t="shared" ref="O8" si="6">N8/1000</f>
         <v>0.28599999999999998</v>
       </c>
-      <c r="P8" s="115">
+      <c r="P8" s="114">
         <f t="shared" si="3"/>
         <v>20.428571428571427</v>
       </c>
-      <c r="Q8" s="115">
+      <c r="Q8" s="114">
         <f t="shared" si="4"/>
         <v>2.0428571428571428E-2</v>
       </c>
@@ -14990,15 +14991,15 @@
       <c r="T8" s="83" t="s">
         <v>245</v>
       </c>
-      <c r="U8" s="125" t="s">
+      <c r="U8" s="124" t="s">
         <v>249</v>
       </c>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
+      <c r="V8" s="124"/>
+      <c r="W8" s="124"/>
       <c r="X8" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="Y8" s="113"/>
+      <c r="Y8" s="112"/>
     </row>
     <row r="9" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -15040,19 +15041,19 @@
       <c r="M9" s="1">
         <v>1</v>
       </c>
-      <c r="N9" s="115">
+      <c r="N9" s="114">
         <f t="shared" ref="N9:N10" si="7">H9+I9+J9+K9+L9+M9</f>
         <v>258</v>
       </c>
-      <c r="O9" s="115">
+      <c r="O9" s="114">
         <f t="shared" ref="O9:O10" si="8">N9/1000</f>
         <v>0.25800000000000001</v>
       </c>
-      <c r="P9" s="115">
+      <c r="P9" s="114">
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="Q9" s="115">
+      <c r="Q9" s="114">
         <f t="shared" si="4"/>
         <v>8.6000000000000007E-2</v>
       </c>
@@ -15065,15 +15066,15 @@
       <c r="T9" s="83" t="s">
         <v>264</v>
       </c>
-      <c r="U9" s="125" t="s">
+      <c r="U9" s="124" t="s">
         <v>265</v>
       </c>
-      <c r="V9" s="125"/>
-      <c r="W9" s="125"/>
+      <c r="V9" s="124"/>
+      <c r="W9" s="124"/>
       <c r="X9" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="Y9" s="112" t="s">
+      <c r="Y9" s="111" t="s">
         <v>267</v>
       </c>
     </row>
@@ -15117,19 +15118,19 @@
       <c r="M10" s="1">
         <v>2</v>
       </c>
-      <c r="N10" s="115">
+      <c r="N10" s="114">
         <f t="shared" si="7"/>
         <v>332</v>
       </c>
-      <c r="O10" s="115">
+      <c r="O10" s="114">
         <f t="shared" si="8"/>
         <v>0.33200000000000002</v>
       </c>
-      <c r="P10" s="115">
+      <c r="P10" s="114">
         <f t="shared" si="3"/>
         <v>19.529411764705884</v>
       </c>
-      <c r="Q10" s="115">
+      <c r="Q10" s="114">
         <f t="shared" si="4"/>
         <v>1.9529411764705882E-2</v>
       </c>
@@ -15142,15 +15143,15 @@
       <c r="T10" s="83" t="s">
         <v>269</v>
       </c>
-      <c r="U10" s="125" t="s">
+      <c r="U10" s="124" t="s">
         <v>268</v>
       </c>
-      <c r="V10" s="125"/>
-      <c r="W10" s="125"/>
+      <c r="V10" s="124"/>
+      <c r="W10" s="124"/>
       <c r="X10" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Y10" s="113"/>
+      <c r="Y10" s="112"/>
     </row>
     <row r="11" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -15192,19 +15193,19 @@
       <c r="M11" s="1">
         <v>1</v>
       </c>
-      <c r="N11" s="115">
+      <c r="N11" s="114">
         <f t="shared" ref="N11" si="9">H11+I11+J11+K11+L11+M11</f>
         <v>89</v>
       </c>
-      <c r="O11" s="115">
+      <c r="O11" s="114">
         <f t="shared" ref="O11" si="10">N11/1000</f>
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="P11" s="115">
+      <c r="P11" s="114">
         <f t="shared" si="3"/>
         <v>22.25</v>
       </c>
-      <c r="Q11" s="115">
+      <c r="Q11" s="114">
         <f t="shared" si="4"/>
         <v>2.2249999999999999E-2</v>
       </c>
@@ -15217,11 +15218,11 @@
       <c r="T11" s="83" t="s">
         <v>279</v>
       </c>
-      <c r="U11" s="125" t="s">
+      <c r="U11" s="124" t="s">
         <v>280</v>
       </c>
-      <c r="V11" s="125"/>
-      <c r="W11" s="125"/>
+      <c r="V11" s="124"/>
+      <c r="W11" s="124"/>
       <c r="X11" s="1" t="s">
         <v>285</v>
       </c>
@@ -15269,19 +15270,19 @@
       <c r="M12" s="1">
         <v>2</v>
       </c>
-      <c r="N12" s="115">
+      <c r="N12" s="114">
         <f t="shared" ref="N12:N13" si="11">H12+I12+J12+K12+L12+M12</f>
         <v>285</v>
       </c>
-      <c r="O12" s="115">
+      <c r="O12" s="114">
         <f t="shared" ref="O12:O13" si="12">N12/1000</f>
         <v>0.28499999999999998</v>
       </c>
-      <c r="P12" s="115">
+      <c r="P12" s="114">
         <f t="shared" si="3"/>
         <v>23.75</v>
       </c>
-      <c r="Q12" s="115">
+      <c r="Q12" s="114">
         <f t="shared" si="4"/>
         <v>2.3749999999999997E-2</v>
       </c>
@@ -15294,11 +15295,11 @@
       <c r="T12" s="83" t="s">
         <v>288</v>
       </c>
-      <c r="U12" s="125" t="s">
+      <c r="U12" s="124" t="s">
         <v>289</v>
       </c>
-      <c r="V12" s="125"/>
-      <c r="W12" s="125"/>
+      <c r="V12" s="124"/>
+      <c r="W12" s="124"/>
       <c r="X12" s="1" t="s">
         <v>290</v>
       </c>
@@ -15344,19 +15345,19 @@
       <c r="M13" s="1">
         <v>0</v>
       </c>
-      <c r="N13" s="115">
+      <c r="N13" s="114">
         <f t="shared" si="11"/>
         <v>87</v>
       </c>
-      <c r="O13" s="115">
+      <c r="O13" s="114">
         <f t="shared" si="12"/>
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="P13" s="115">
+      <c r="P13" s="114">
         <f t="shared" si="3"/>
         <v>21.75</v>
       </c>
-      <c r="Q13" s="115">
+      <c r="Q13" s="114">
         <f t="shared" si="4"/>
         <v>2.1749999999999999E-2</v>
       </c>
@@ -15369,15 +15370,15 @@
       <c r="T13" s="83" t="s">
         <v>302</v>
       </c>
-      <c r="U13" s="125" t="s">
+      <c r="U13" s="124" t="s">
         <v>303</v>
       </c>
-      <c r="V13" s="125"/>
-      <c r="W13" s="125"/>
+      <c r="V13" s="124"/>
+      <c r="W13" s="124"/>
       <c r="X13" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="Y13" s="112" t="s">
+      <c r="Y13" s="111" t="s">
         <v>307</v>
       </c>
     </row>
@@ -15421,19 +15422,19 @@
       <c r="M14" s="1">
         <v>1</v>
       </c>
-      <c r="N14" s="115">
+      <c r="N14" s="114">
         <f t="shared" ref="N14:N23" si="13">H14+I14+J14+K14+L14+M14</f>
         <v>317</v>
       </c>
-      <c r="O14" s="115">
+      <c r="O14" s="114">
         <f t="shared" ref="O14:O23" si="14">N14/1000</f>
         <v>0.317</v>
       </c>
-      <c r="P14" s="115">
+      <c r="P14" s="114">
         <f t="shared" si="3"/>
         <v>18.647058823529413</v>
       </c>
-      <c r="Q14" s="115">
+      <c r="Q14" s="114">
         <f t="shared" si="4"/>
         <v>1.8647058823529412E-2</v>
       </c>
@@ -15446,15 +15447,15 @@
       <c r="T14" s="83" t="s">
         <v>309</v>
       </c>
-      <c r="U14" s="125" t="s">
+      <c r="U14" s="124" t="s">
         <v>308</v>
       </c>
-      <c r="V14" s="125"/>
-      <c r="W14" s="125"/>
+      <c r="V14" s="124"/>
+      <c r="W14" s="124"/>
       <c r="X14" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Y14" s="113"/>
+      <c r="Y14" s="112"/>
     </row>
     <row r="15" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -15496,19 +15497,19 @@
       <c r="M15" s="1">
         <v>1</v>
       </c>
-      <c r="N15" s="115">
+      <c r="N15" s="114">
         <f t="shared" si="13"/>
         <v>123</v>
       </c>
-      <c r="O15" s="115">
+      <c r="O15" s="114">
         <f t="shared" si="14"/>
         <v>0.123</v>
       </c>
-      <c r="P15" s="115">
+      <c r="P15" s="114">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="Q15" s="115">
+      <c r="Q15" s="114">
         <f t="shared" si="4"/>
         <v>4.1000000000000002E-2</v>
       </c>
@@ -15521,15 +15522,15 @@
       <c r="T15" s="83" t="s">
         <v>311</v>
       </c>
-      <c r="U15" s="125" t="s">
+      <c r="U15" s="124" t="s">
         <v>312</v>
       </c>
-      <c r="V15" s="125"/>
-      <c r="W15" s="125"/>
+      <c r="V15" s="124"/>
+      <c r="W15" s="124"/>
       <c r="X15" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="Y15" s="112" t="s">
+      <c r="Y15" s="111" t="s">
         <v>316</v>
       </c>
     </row>
@@ -15573,19 +15574,19 @@
       <c r="M16" s="1">
         <v>2</v>
       </c>
-      <c r="N16" s="115">
+      <c r="N16" s="114">
         <f t="shared" si="13"/>
         <v>232</v>
       </c>
-      <c r="O16" s="115">
+      <c r="O16" s="114">
         <f t="shared" si="14"/>
         <v>0.23200000000000001</v>
       </c>
-      <c r="P16" s="115">
+      <c r="P16" s="114">
         <f t="shared" si="3"/>
         <v>21.09090909090909</v>
       </c>
-      <c r="Q16" s="115">
+      <c r="Q16" s="114">
         <f t="shared" si="4"/>
         <v>2.1090909090909091E-2</v>
       </c>
@@ -15598,15 +15599,15 @@
       <c r="T16" s="83" t="s">
         <v>318</v>
       </c>
-      <c r="U16" s="125" t="s">
+      <c r="U16" s="124" t="s">
         <v>317</v>
       </c>
-      <c r="V16" s="125"/>
-      <c r="W16" s="125"/>
+      <c r="V16" s="124"/>
+      <c r="W16" s="124"/>
       <c r="X16" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="Y16" s="113"/>
+      <c r="Y16" s="112"/>
     </row>
     <row r="17" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -15648,19 +15649,19 @@
       <c r="M17" s="1">
         <v>2</v>
       </c>
-      <c r="N17" s="115">
+      <c r="N17" s="114">
         <f t="shared" si="13"/>
         <v>134</v>
       </c>
-      <c r="O17" s="115">
+      <c r="O17" s="114">
         <f t="shared" si="14"/>
         <v>0.13400000000000001</v>
       </c>
-      <c r="P17" s="115">
+      <c r="P17" s="114">
         <f t="shared" si="3"/>
         <v>33.5</v>
       </c>
-      <c r="Q17" s="115">
+      <c r="Q17" s="114">
         <f t="shared" si="4"/>
         <v>3.3500000000000002E-2</v>
       </c>
@@ -15673,15 +15674,15 @@
       <c r="T17" s="83" t="s">
         <v>336</v>
       </c>
-      <c r="U17" s="133" t="s">
+      <c r="U17" s="132" t="s">
         <v>337</v>
       </c>
-      <c r="V17" s="134"/>
+      <c r="V17" s="133"/>
       <c r="W17" s="10"/>
       <c r="X17" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="Y17" s="112" t="s">
+      <c r="Y17" s="111" t="s">
         <v>341</v>
       </c>
     </row>
@@ -15725,19 +15726,19 @@
       <c r="M18" s="1">
         <v>4</v>
       </c>
-      <c r="N18" s="115">
+      <c r="N18" s="114">
         <f t="shared" si="13"/>
         <v>240</v>
       </c>
-      <c r="O18" s="115">
+      <c r="O18" s="114">
         <f t="shared" si="14"/>
         <v>0.24</v>
       </c>
-      <c r="P18" s="115">
+      <c r="P18" s="114">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="Q18" s="115">
+      <c r="Q18" s="114">
         <f t="shared" si="4"/>
         <v>2.4E-2</v>
       </c>
@@ -15750,15 +15751,15 @@
       <c r="T18" s="83" t="s">
         <v>343</v>
       </c>
-      <c r="U18" s="135" t="s">
+      <c r="U18" s="134" t="s">
         <v>342</v>
       </c>
-      <c r="V18" s="136"/>
+      <c r="V18" s="135"/>
       <c r="W18" s="10"/>
       <c r="X18" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="Y18" s="113"/>
+      <c r="Y18" s="112"/>
     </row>
     <row r="19" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -15800,19 +15801,19 @@
       <c r="M19" s="1">
         <v>1</v>
       </c>
-      <c r="N19" s="115">
+      <c r="N19" s="114">
         <f t="shared" si="13"/>
         <v>68</v>
       </c>
-      <c r="O19" s="115">
+      <c r="O19" s="114">
         <f t="shared" si="14"/>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="P19" s="115">
+      <c r="P19" s="114">
         <f t="shared" si="3"/>
         <v>13.6</v>
       </c>
-      <c r="Q19" s="115">
+      <c r="Q19" s="114">
         <f t="shared" si="4"/>
         <v>1.3600000000000001E-2</v>
       </c>
@@ -15825,15 +15826,15 @@
       <c r="T19" s="83" t="s">
         <v>356</v>
       </c>
-      <c r="U19" s="135" t="s">
+      <c r="U19" s="134" t="s">
         <v>355</v>
       </c>
-      <c r="V19" s="136"/>
+      <c r="V19" s="135"/>
       <c r="W19" s="10"/>
       <c r="X19" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="Y19" s="112" t="s">
+      <c r="Y19" s="111" t="s">
         <v>360</v>
       </c>
     </row>
@@ -15877,19 +15878,19 @@
       <c r="M20" s="1">
         <v>2</v>
       </c>
-      <c r="N20" s="115">
+      <c r="N20" s="114">
         <f t="shared" si="13"/>
         <v>310</v>
       </c>
-      <c r="O20" s="115">
+      <c r="O20" s="114">
         <f t="shared" si="14"/>
         <v>0.31</v>
       </c>
-      <c r="P20" s="115">
+      <c r="P20" s="114">
         <f t="shared" si="3"/>
         <v>15.5</v>
       </c>
-      <c r="Q20" s="115">
+      <c r="Q20" s="114">
         <f t="shared" si="4"/>
         <v>1.55E-2</v>
       </c>
@@ -15902,15 +15903,15 @@
       <c r="T20" s="83" t="s">
         <v>362</v>
       </c>
-      <c r="U20" s="135" t="s">
+      <c r="U20" s="134" t="s">
         <v>361</v>
       </c>
-      <c r="V20" s="136"/>
+      <c r="V20" s="135"/>
       <c r="W20" s="10"/>
       <c r="X20" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="Y20" s="113"/>
+      <c r="Y20" s="112"/>
     </row>
     <row r="21" spans="1:25" s="67" customFormat="1" ht="378" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -15952,19 +15953,19 @@
       <c r="M21" s="1">
         <v>0</v>
       </c>
-      <c r="N21" s="115">
+      <c r="N21" s="114">
         <f t="shared" si="13"/>
         <v>76</v>
       </c>
-      <c r="O21" s="115">
+      <c r="O21" s="114">
         <f t="shared" si="14"/>
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="P21" s="115">
+      <c r="P21" s="114">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="Q21" s="115">
+      <c r="Q21" s="114">
         <f t="shared" si="4"/>
         <v>1.9E-2</v>
       </c>
@@ -15977,10 +15978,10 @@
       <c r="T21" s="83" t="s">
         <v>375</v>
       </c>
-      <c r="U21" s="133" t="s">
+      <c r="U21" s="132" t="s">
         <v>376</v>
       </c>
-      <c r="V21" s="134"/>
+      <c r="V21" s="133"/>
       <c r="W21" s="10"/>
       <c r="X21" s="1" t="s">
         <v>377</v>
@@ -16029,19 +16030,19 @@
       <c r="M22" s="1">
         <v>0</v>
       </c>
-      <c r="N22" s="115">
+      <c r="N22" s="114">
         <f t="shared" si="13"/>
         <v>157</v>
       </c>
-      <c r="O22" s="115">
+      <c r="O22" s="114">
         <f t="shared" si="14"/>
         <v>0.157</v>
       </c>
-      <c r="P22" s="115">
+      <c r="P22" s="114">
         <f t="shared" si="3"/>
         <v>19.625</v>
       </c>
-      <c r="Q22" s="115">
+      <c r="Q22" s="114">
         <f t="shared" si="4"/>
         <v>1.9625E-2</v>
       </c>
@@ -16054,10 +16055,10 @@
       <c r="T22" s="83" t="s">
         <v>382</v>
       </c>
-      <c r="U22" s="133" t="s">
+      <c r="U22" s="132" t="s">
         <v>381</v>
       </c>
-      <c r="V22" s="134"/>
+      <c r="V22" s="133"/>
       <c r="W22" s="10"/>
       <c r="X22" s="1" t="s">
         <v>383</v>
@@ -16104,19 +16105,19 @@
       <c r="M23" s="1">
         <v>0</v>
       </c>
-      <c r="N23" s="115">
+      <c r="N23" s="114">
         <f t="shared" si="13"/>
         <v>24</v>
       </c>
-      <c r="O23" s="115">
+      <c r="O23" s="114">
         <f t="shared" si="14"/>
         <v>2.4E-2</v>
       </c>
-      <c r="P23" s="115">
+      <c r="P23" s="114">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="Q23" s="115">
+      <c r="Q23" s="114">
         <f t="shared" si="4"/>
         <v>2.4E-2</v>
       </c>
@@ -16129,15 +16130,15 @@
       <c r="T23" s="83" t="s">
         <v>324</v>
       </c>
-      <c r="U23" s="125" t="s">
+      <c r="U23" s="124" t="s">
         <v>325</v>
       </c>
-      <c r="V23" s="125"/>
-      <c r="W23" s="125"/>
+      <c r="V23" s="124"/>
+      <c r="W23" s="124"/>
       <c r="X23" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="Y23" s="112" t="s">
+      <c r="Y23" s="111" t="s">
         <v>333</v>
       </c>
     </row>
@@ -16181,19 +16182,19 @@
       <c r="M24" s="1">
         <v>0</v>
       </c>
-      <c r="N24" s="115">
+      <c r="N24" s="114">
         <f t="shared" ref="N24:N26" si="15">H24+I24+J24+K24+L24+M24</f>
         <v>14</v>
       </c>
-      <c r="O24" s="115">
+      <c r="O24" s="114">
         <f t="shared" ref="O24:O26" si="16">N24/1000</f>
         <v>1.4E-2</v>
       </c>
-      <c r="P24" s="115">
+      <c r="P24" s="114">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="Q24" s="115">
+      <c r="Q24" s="114">
         <f t="shared" si="4"/>
         <v>1.4E-2</v>
       </c>
@@ -16206,15 +16207,15 @@
       <c r="T24" s="83" t="s">
         <v>324</v>
       </c>
-      <c r="U24" s="125" t="s">
+      <c r="U24" s="124" t="s">
         <v>325</v>
       </c>
-      <c r="V24" s="125"/>
-      <c r="W24" s="125"/>
+      <c r="V24" s="124"/>
+      <c r="W24" s="124"/>
       <c r="X24" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="Y24" s="113"/>
+      <c r="Y24" s="112"/>
     </row>
     <row r="25" spans="1:25" s="67" customFormat="1" ht="268" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
@@ -16256,19 +16257,19 @@
       <c r="M25" s="1">
         <v>0</v>
       </c>
-      <c r="N25" s="115">
+      <c r="N25" s="114">
         <f t="shared" si="15"/>
         <v>19</v>
       </c>
-      <c r="O25" s="115">
+      <c r="O25" s="114">
         <f t="shared" si="16"/>
         <v>1.9E-2</v>
       </c>
-      <c r="P25" s="115">
+      <c r="P25" s="114">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="Q25" s="115">
+      <c r="Q25" s="114">
         <f t="shared" si="4"/>
         <v>1.9E-2</v>
       </c>
@@ -16281,15 +16282,15 @@
       <c r="T25" s="83" t="s">
         <v>327</v>
       </c>
-      <c r="U25" s="125" t="s">
+      <c r="U25" s="124" t="s">
         <v>328</v>
       </c>
-      <c r="V25" s="125"/>
-      <c r="W25" s="125"/>
+      <c r="V25" s="124"/>
+      <c r="W25" s="124"/>
       <c r="X25" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="Y25" s="112" t="s">
+      <c r="Y25" s="111" t="s">
         <v>332</v>
       </c>
     </row>
@@ -16333,19 +16334,19 @@
       <c r="M26" s="1">
         <v>0</v>
       </c>
-      <c r="N26" s="115">
+      <c r="N26" s="114">
         <f t="shared" si="15"/>
         <v>22</v>
       </c>
-      <c r="O26" s="115">
+      <c r="O26" s="114">
         <f t="shared" si="16"/>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="P26" s="115">
+      <c r="P26" s="114">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="Q26" s="115">
+      <c r="Q26" s="114">
         <f t="shared" si="4"/>
         <v>2.1999999999999999E-2</v>
       </c>
@@ -16358,15 +16359,15 @@
       <c r="T26" s="83" t="s">
         <v>327</v>
       </c>
-      <c r="U26" s="125" t="s">
+      <c r="U26" s="124" t="s">
         <v>328</v>
       </c>
-      <c r="V26" s="125"/>
-      <c r="W26" s="125"/>
+      <c r="V26" s="124"/>
+      <c r="W26" s="124"/>
       <c r="X26" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="Y26" s="113"/>
+      <c r="Y26" s="112"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Y26" xr:uid="{479C7C77-DD3E-B144-B850-10F0059BAEDA}">
@@ -16518,7 +16519,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="110" t="s">
         <v>410</v>
       </c>
@@ -16528,7 +16529,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="110" t="s">
         <v>411</v>
       </c>
@@ -16538,7 +16539,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="110" t="s">
         <v>413</v>
       </c>
@@ -16548,7 +16549,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="110" t="s">
         <v>415</v>
       </c>

</xml_diff>